<commit_message>
working notebook for 5 datasets 2017 and 2018 harvest
</commit_message>
<xml_diff>
--- a/data/raw/April_2017.xlsx
+++ b/data/raw/April_2017.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\FCSC\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\FSCS_Project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED7BD8E-3D63-45AF-A299-AE48D506B382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CF6A20-D2FF-48A0-A753-811CE92489E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20505" yWindow="2205" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19980" yWindow="2100" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="28">
   <si>
     <t>Timestamp</t>
   </si>
   <si>
     <t>Strain</t>
-  </si>
-  <si>
-    <t>Plant #</t>
   </si>
   <si>
     <t>Trimmer</t>
@@ -384,9 +381,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Justin" refreshedDate="44802.518200925922" refreshedVersion="8" recordCount="146" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Justin" refreshedDate="44802.725721527779" refreshedVersion="8" recordCount="146" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:E1146" sheet="Form Responses 1"/>
+    <worksheetSource ref="B1:D1146" sheet="Form Responses 1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Strain" numFmtId="0">
@@ -2183,19 +2180,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="18.85546875" customWidth="1"/>
+    <col min="1" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2205,1466 +2202,1381 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-    </row>
-    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>42843.447165891208</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E84" s="1">
+      <c r="D84" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>42843.447581469911</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85" s="1">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="1">
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>42843.543546701389</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="1">
+        <v>4</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>42843.543720069443</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E87" s="1">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>42843.54853137731</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E88" s="1">
+      <c r="D88" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>42843.631073101853</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" s="1">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>42843.631316874998</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E90" s="1">
+        <v>4</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>42843.63466787037</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E91" s="1">
+      <c r="D91" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>42843.666363946759</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="1">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>42843.666598402779</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="1">
+      <c r="D93" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>42843.81642052083</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E94" s="1">
+        <v>4</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>42843.834654791666</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95" s="1">
+      <c r="D95" s="1">
         <v>25.3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>42843.941048298613</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="1">
+      <c r="C96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="1">
         <v>30.8</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>42843.941238067127</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="1">
+      <c r="C97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>42843.948303472222</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" s="1">
+        <v>7</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="1">
         <v>19.5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>42844.939043449078</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="1">
+      <c r="C99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>42844.939987303238</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="1">
+        <v>8</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" s="1">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>42845.514080335648</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="1">
+        <v>7</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="1">
         <v>25.6</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>42845.514591180559</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E102" s="1">
+      <c r="C102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>42845.518218715282</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="1">
+        <v>8</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>42845.519680833335</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="1">
+        <v>8</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>42845.642532916667</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E105" s="1">
+        <v>8</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>42845.938595219908</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E106" s="1">
+      <c r="D106" s="1">
         <v>7.3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>42847.673560601848</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D107" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E107" s="1">
+      <c r="C107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>42847.674513171296</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E108" s="1">
+        <v>10</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>42847.962356782409</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E109" s="1">
+      <c r="D109" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>42847.963524282408</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="1">
+        <v>8</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>42847.964515115746</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E111" s="1">
+        <v>8</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>42847.965166817128</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D112" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E112" s="1">
+      <c r="C112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>42847.966358958336</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E113" s="1">
+        <v>10</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="1">
         <v>44.5</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>42847.966868819443</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E114" s="1">
+      <c r="D114" s="1">
         <v>19.5</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>42847.967685243057</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E115" s="1">
+        <v>10</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>42847.968193125002</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" s="1">
+        <v>10</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="1">
         <v>39.5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>42847.968816886569</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E117" s="1">
+        <v>10</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117" s="1">
         <v>127.5</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>42847.969639710645</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E118" s="1">
+        <v>7</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>42847.9705583912</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" s="1">
+        <v>7</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>42847.970982870371</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E120" s="1">
+        <v>7</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" s="1">
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>42848.038560787041</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D121" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E121" s="1">
+      <c r="C121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="1">
         <v>38.1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>42848.0399396875</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E122" s="1">
+        <v>13</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" s="1">
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>42848.668904618055</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E123" s="1">
+      <c r="D123" s="1">
         <v>50.3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>42848.670183657407</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E124" s="1">
+        <v>14</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" s="1">
         <v>49.8</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>42850.084939004628</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E125" s="1">
+        <v>17</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>42850.11060443287</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E126" s="1">
+        <v>17</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" s="1">
         <v>87</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>42850.111446296301</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" s="1">
+        <v>17</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="1">
         <v>132.5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>42850.112652071759</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E128" s="1">
+        <v>14</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>42850.115003993051</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E129" s="1">
+        <v>14</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D129" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>42850.990525405097</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E130" s="1">
+        <v>17</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>42855.038524340278</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E131" s="1">
+        <v>7</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>42855.039635972222</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E132" s="1">
+        <v>7</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D132" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>42855.04041306713</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>42855.041337013885</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E134" s="1">
+        <v>8</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>42856.409261284723</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E135" s="1">
+        <v>10</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>42856.409548090276</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D136" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="1">
         <v>7</v>
       </c>
-      <c r="E136" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>42856.409940949074</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E137" s="1">
+        <v>8</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D137" s="1">
         <v>47.5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>42856.41072565972</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E138" s="1">
+        <v>7</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D138" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>42856.411417986106</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E139" s="1">
+        <v>7</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139" s="1">
         <v>42.5</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>42856.411837037042</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E140" s="1">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>42856.412845208339</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E141" s="1">
+      <c r="D141" s="1">
         <v>98</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>42856.413590138887</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E142" s="1">
+        <v>8</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>42856.415663958338</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E143" s="1">
+      <c r="D143" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>42856.416400000002</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E144" s="1">
+        <v>10</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" s="1">
         <v>77.5</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>42856.417996412041</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E145" s="1">
+        <v>7</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D145" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>42856.418145069445</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E146" s="1">
+        <v>7</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" s="1">
         <v>55</v>
       </c>
     </row>
@@ -3687,100 +3599,100 @@
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="16"/>
       <c r="H1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="16"/>
       <c r="J1" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="16"/>
       <c r="N1" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="16"/>
       <c r="R1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R2" s="19"/>
       <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22">
@@ -3825,7 +3737,7 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="25">
         <v>127.5</v>
@@ -3878,7 +3790,7 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="25">
         <v>117.5</v>
@@ -3925,7 +3837,7 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="25">
         <v>97.5</v>
@@ -3980,7 +3892,7 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="25">
         <v>36</v>
@@ -4031,7 +3943,7 @@
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26">
@@ -4076,7 +3988,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="26">
@@ -4121,7 +4033,7 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="25">
         <v>267</v>
@@ -4178,7 +4090,7 @@
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="26">
@@ -4223,7 +4135,7 @@
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="26">
@@ -4264,7 +4176,7 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="29">
         <v>645.5</v>
@@ -4338,120 +4250,120 @@
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="16"/>
       <c r="H1" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="16"/>
       <c r="J1" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" s="16"/>
       <c r="N1" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q1" s="16"/>
       <c r="R1" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S1" s="16"/>
       <c r="T1" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U1" s="16"/>
       <c r="V1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V2" s="19"/>
       <c r="W2" s="20"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22">
@@ -4512,7 +4424,7 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="26">
@@ -4575,7 +4487,7 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="25">
         <v>49.8</v>
@@ -4634,7 +4546,7 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="26">
@@ -4691,7 +4603,7 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="26">
@@ -4750,7 +4662,7 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26">
@@ -4805,7 +4717,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="26">
@@ -4864,7 +4776,7 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="26">
@@ -4913,7 +4825,7 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="29">
         <v>49.8</v>
@@ -5013,100 +4925,100 @@
     <row r="1" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="16"/>
       <c r="H1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="16"/>
       <c r="J1" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="16"/>
       <c r="N1" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1" s="16"/>
       <c r="P1" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="16"/>
       <c r="R1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R2" s="19"/>
       <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22">
@@ -5151,7 +5063,7 @@
     </row>
     <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="25">
         <v>127.5</v>
@@ -5204,7 +5116,7 @@
     </row>
     <row r="5" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="25">
         <v>117.5</v>
@@ -5251,7 +5163,7 @@
     </row>
     <row r="6" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="25">
         <v>97.5</v>
@@ -5306,7 +5218,7 @@
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="25">
         <v>36</v>
@@ -5375,7 +5287,7 @@
     </row>
     <row r="8" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26">
@@ -5420,7 +5332,7 @@
     </row>
     <row r="9" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="26">
@@ -5465,7 +5377,7 @@
     </row>
     <row r="10" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="25">
         <v>267</v>
@@ -5540,7 +5452,7 @@
     </row>
     <row r="11" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="26">
@@ -5603,7 +5515,7 @@
     </row>
     <row r="12" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="26">
@@ -5644,7 +5556,7 @@
     </row>
     <row r="13" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="29">
         <v>645.5</v>
@@ -19540,24 +19452,24 @@
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="20"/>
@@ -19565,7 +19477,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="21">
         <v>645.5</v>
@@ -19583,7 +19495,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="25">
         <v>893.4</v>
@@ -19601,7 +19513,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="25">
         <v>386.1</v>
@@ -19619,7 +19531,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="25">
         <v>458.5</v>
@@ -19637,7 +19549,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="25">
         <v>519.5</v>
@@ -19655,7 +19567,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="25">
         <v>56.2</v>
@@ -19673,7 +19585,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="25">
         <v>644.29999999999995</v>
@@ -19691,7 +19603,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="26">
@@ -19705,7 +19617,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="29">
         <v>3603.5</v>

</xml_diff>